<commit_message>
- added CSV support - added sqlite example - adjusted xlsx to import template from samedis.care - allow optional fields
</commit_message>
<xml_diff>
--- a/import/import.xlsx
+++ b/import/import.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yvesrausch/github/samedis-care-staff-sync/import/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17A8090-F2F7-BA42-AB1E-0A672ED3A883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A1860B-65EF-EC41-8FE1-64FDF771AB16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-42060" yWindow="-1480" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,15 +41,6 @@
     <t>Vorname</t>
   </si>
   <si>
-    <t>Personalnummer</t>
-  </si>
-  <si>
-    <t>Eintrittsdatum</t>
-  </si>
-  <si>
-    <t>Austrittsdatum</t>
-  </si>
-  <si>
     <t>E-Mail</t>
   </si>
   <si>
@@ -75,6 +66,15 @@
   </si>
   <si>
     <t>0151 123456789</t>
+  </si>
+  <si>
+    <t>Mitarbeiternr.</t>
+  </si>
+  <si>
+    <t>Austritt am</t>
+  </si>
+  <si>
+    <t>Beitritt am</t>
   </si>
 </sst>
 </file>
@@ -456,7 +456,7 @@
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -472,33 +472,33 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C2">
         <v>12345</v>
@@ -512,13 +512,13 @@
         <v>NachnameBeispiel.VornameBeispiel@domain.local</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="I2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">

</xml_diff>